<commit_message>
Elimina archivos de datos, añade datos para prueba de dos días
</commit_message>
<xml_diff>
--- a/Audios/TwoDayProtocol/Lista de estímulos.xlsx
+++ b/Audios/TwoDayProtocol/Lista de estímulos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\jmriv\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\jmriv\Documents\GitHub\cajaSobresaltoArduino\Audios\TwoDayProtocol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D5ECD9-E1DB-4A54-9F54-CAF1D9E83EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC61CB33-7118-43A4-BDFD-A9AC1A1465AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D0241131-5F6E-5641-B73B-EA17B42B127C}"/>
+    <workbookView xWindow="-120" yWindow="4710" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{D0241131-5F6E-5641-B73B-EA17B42B127C}"/>
   </bookViews>
   <sheets>
     <sheet name="Día 1" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="37">
   <si>
     <t>tiempo</t>
   </si>
@@ -166,6 +166,12 @@
   </si>
   <si>
     <t>identificación</t>
+  </si>
+  <si>
+    <t>Background</t>
+  </si>
+  <si>
+    <t>65 dB</t>
   </si>
 </sst>
 </file>
@@ -210,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -232,6 +238,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,293 +553,341 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BA065A2-5DC2-8940-8ADE-B1B90323E971}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="TU1" zoomScale="91" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView zoomScale="91" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="1"/>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="C3">
         <v>76</v>
       </c>
-      <c r="C2">
-        <f>HOUR(A2)</f>
+      <c r="D3">
+        <f>HOUR(B3)</f>
         <v>5</v>
       </c>
-      <c r="D2">
-        <f>MINUTE(A2)</f>
+      <c r="E3">
+        <f>MINUTE(B3)</f>
         <v>12</v>
       </c>
-      <c r="E2">
-        <f>C2*60*1000+D2*1000</f>
+      <c r="F3">
+        <f>D3*60*1000+E3*1000</f>
         <v>312000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
-        <f>B2+2</f>
+      <c r="C4">
+        <f>C3+2</f>
         <v>78</v>
       </c>
-      <c r="C3">
-        <f t="shared" ref="C3:C14" si="0">HOUR(A3)</f>
+      <c r="D4">
+        <f t="shared" ref="D4:D15" si="0">HOUR(B4)</f>
         <v>5</v>
       </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D14" si="1">MINUTE(A3)</f>
+      <c r="E4">
+        <f t="shared" ref="E4:E15" si="1">MINUTE(B4)</f>
         <v>22</v>
       </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E14" si="2">C3*60*1000+D3*1000</f>
+      <c r="F4">
+        <f t="shared" ref="F4:F15" si="2">D4*60*1000+E4*1000</f>
         <v>322000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
-        <f t="shared" ref="B4:B14" si="3">B3+2</f>
+      <c r="C5">
+        <f t="shared" ref="C5:C15" si="3">C4+2</f>
         <v>80</v>
       </c>
-      <c r="C4">
+      <c r="D5">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D4">
+      <c r="E5">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="E4">
+      <c r="F5">
         <f t="shared" si="2"/>
         <v>332000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="C6">
         <f t="shared" si="3"/>
         <v>82</v>
       </c>
-      <c r="C5">
+      <c r="D6">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D5">
+      <c r="E6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E5">
+      <c r="F6">
         <f t="shared" si="2"/>
         <v>360000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="C7">
         <f t="shared" si="3"/>
         <v>84</v>
       </c>
-      <c r="C6">
+      <c r="D7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D6">
+      <c r="E7">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="E6">
+      <c r="F7">
         <f t="shared" si="2"/>
         <v>379000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
+      <c r="C8">
         <f t="shared" si="3"/>
         <v>86</v>
       </c>
-      <c r="C7">
+      <c r="D8">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D7">
+      <c r="E8">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="E7">
+      <c r="F8">
         <f t="shared" si="2"/>
         <v>401000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B8">
+      <c r="C9">
         <f t="shared" si="3"/>
         <v>88</v>
       </c>
-      <c r="C8">
+      <c r="D9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="D8">
+      <c r="E9">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="E8">
+      <c r="F9">
         <f t="shared" si="2"/>
         <v>433000</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B9">
+      <c r="C10">
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
-      <c r="C9">
+      <c r="D10">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="D9">
+      <c r="E10">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="E9">
+      <c r="F10">
         <f t="shared" si="2"/>
         <v>462000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10">
+      <c r="C11">
         <f t="shared" si="3"/>
         <v>92</v>
       </c>
-      <c r="C10">
+      <c r="D11">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="D10">
+      <c r="E11">
         <f t="shared" si="1"/>
         <v>59</v>
       </c>
-      <c r="E10">
+      <c r="F11">
         <f t="shared" si="2"/>
         <v>479000</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B11">
+      <c r="C12">
         <f t="shared" si="3"/>
         <v>94</v>
       </c>
-      <c r="C11">
+      <c r="D12">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="D11">
+      <c r="E12">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="E11">
+      <c r="F12">
         <f t="shared" si="2"/>
         <v>495000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B12">
+      <c r="C13">
         <f t="shared" si="3"/>
         <v>96</v>
       </c>
-      <c r="C12">
+      <c r="D13">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="D12">
+      <c r="E13">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="E12">
+      <c r="F13">
         <f t="shared" si="2"/>
         <v>509000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B13">
+      <c r="C14">
         <f t="shared" si="3"/>
         <v>98</v>
       </c>
-      <c r="C13">
+      <c r="D14">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="D13">
+      <c r="E14">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="E13">
+      <c r="F14">
         <f t="shared" si="2"/>
         <v>522000</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B14">
+      <c r="C15">
         <f t="shared" si="3"/>
         <v>100</v>
       </c>
-      <c r="C14">
+      <c r="D15">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="D14">
+      <c r="E15">
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
-      <c r="E14">
+      <c r="F15">
         <f t="shared" si="2"/>
         <v>537000</v>
       </c>
@@ -846,12 +901,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F9C66F9-9290-3F4F-AC95-4DC15AA659AC}">
   <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="4.77734375" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" customWidth="1"/>
     <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.88671875" bestFit="1" customWidth="1"/>
@@ -906,6 +962,10 @@
       <c r="F2">
         <v>100</v>
       </c>
+      <c r="G2" s="9">
+        <f>MINUTE(B2)*60*1000+SECOND(B2)*1000</f>
+        <v>300000</v>
+      </c>
       <c r="I2" s="4" t="s">
         <v>30</v>
       </c>
@@ -935,6 +995,10 @@
       <c r="F3">
         <v>100</v>
       </c>
+      <c r="G3" s="9">
+        <f t="shared" ref="G3:G61" si="1">MINUTE(B3)*60*1000+SECOND(B3)*1000</f>
+        <v>315000</v>
+      </c>
       <c r="I3" s="3" t="s">
         <v>20</v>
       </c>
@@ -964,6 +1028,10 @@
       <c r="F4">
         <v>100</v>
       </c>
+      <c r="G4" s="9">
+        <f t="shared" si="1"/>
+        <v>329000</v>
+      </c>
       <c r="I4" s="3" t="s">
         <v>21</v>
       </c>
@@ -993,6 +1061,10 @@
       <c r="F5">
         <v>100</v>
       </c>
+      <c r="G5" s="9">
+        <f t="shared" si="1"/>
+        <v>342000</v>
+      </c>
       <c r="I5" s="3" t="s">
         <v>23</v>
       </c>
@@ -1022,6 +1094,10 @@
       <c r="F6">
         <v>100</v>
       </c>
+      <c r="G6" s="9">
+        <f t="shared" si="1"/>
+        <v>353000</v>
+      </c>
       <c r="I6" s="3" t="s">
         <v>25</v>
       </c>
@@ -1051,6 +1127,10 @@
       <c r="F7">
         <v>100</v>
       </c>
+      <c r="G7" s="9">
+        <f t="shared" si="1"/>
+        <v>368000</v>
+      </c>
       <c r="I7" s="3" t="s">
         <v>26</v>
       </c>
@@ -1080,6 +1160,10 @@
       <c r="F8">
         <v>100</v>
       </c>
+      <c r="G8" s="9">
+        <f t="shared" si="1"/>
+        <v>378000</v>
+      </c>
       <c r="I8" s="3" t="s">
         <v>27</v>
       </c>
@@ -1109,6 +1193,10 @@
       <c r="F9">
         <v>100</v>
       </c>
+      <c r="G9" s="9">
+        <f t="shared" si="1"/>
+        <v>393000</v>
+      </c>
       <c r="I9" s="3" t="s">
         <v>28</v>
       </c>
@@ -1138,6 +1226,10 @@
       <c r="F10">
         <v>100</v>
       </c>
+      <c r="G10" s="9">
+        <f t="shared" si="1"/>
+        <v>403000</v>
+      </c>
       <c r="I10" s="3" t="s">
         <v>29</v>
       </c>
@@ -1167,6 +1259,10 @@
       <c r="F11">
         <v>100</v>
       </c>
+      <c r="G11" s="9">
+        <f t="shared" si="1"/>
+        <v>413000</v>
+      </c>
       <c r="I11" s="4" t="s">
         <v>31</v>
       </c>
@@ -1196,6 +1292,10 @@
       <c r="F12">
         <v>75</v>
       </c>
+      <c r="G12" s="9">
+        <f t="shared" si="1"/>
+        <v>425000</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -1218,6 +1318,10 @@
       <c r="F13">
         <v>75</v>
       </c>
+      <c r="G13" s="9">
+        <f t="shared" si="1"/>
+        <v>439000</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -1240,6 +1344,10 @@
       <c r="F14">
         <v>85</v>
       </c>
+      <c r="G14" s="9">
+        <f t="shared" si="1"/>
+        <v>453000</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -1262,6 +1370,10 @@
       <c r="F15">
         <v>85</v>
       </c>
+      <c r="G15" s="9">
+        <f t="shared" si="1"/>
+        <v>468000</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -1284,8 +1396,12 @@
       <c r="F16">
         <v>100</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" s="9">
+        <f t="shared" si="1"/>
+        <v>483000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1306,8 +1422,12 @@
       <c r="F17">
         <v>85</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" s="9">
+        <f t="shared" si="1"/>
+        <v>495000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1328,8 +1448,12 @@
       <c r="F18">
         <v>85</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" s="9">
+        <f t="shared" si="1"/>
+        <v>505000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1350,8 +1474,12 @@
       <c r="F19">
         <v>75</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" s="9">
+        <f t="shared" si="1"/>
+        <v>516000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1372,8 +1500,12 @@
       <c r="F20">
         <v>75</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" s="9">
+        <f t="shared" si="1"/>
+        <v>526000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1394,8 +1526,12 @@
       <c r="F21">
         <v>85</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21" s="9">
+        <f t="shared" si="1"/>
+        <v>541000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1416,8 +1552,12 @@
       <c r="F22">
         <v>75</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22" s="9">
+        <f t="shared" si="1"/>
+        <v>553000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1438,8 +1578,12 @@
       <c r="F23">
         <v>75</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23" s="9">
+        <f t="shared" si="1"/>
+        <v>566000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1460,8 +1604,12 @@
       <c r="F24">
         <v>75</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24" s="9">
+        <f t="shared" si="1"/>
+        <v>578000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1482,8 +1630,12 @@
       <c r="F25">
         <v>100</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25" s="9">
+        <f t="shared" si="1"/>
+        <v>589000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1504,8 +1656,12 @@
       <c r="F26">
         <v>85</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26" s="9">
+        <f t="shared" si="1"/>
+        <v>601000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1526,8 +1682,12 @@
       <c r="F27">
         <v>85</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27" s="9">
+        <f t="shared" si="1"/>
+        <v>618000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1548,8 +1708,12 @@
       <c r="F28">
         <v>85</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28" s="9">
+        <f t="shared" si="1"/>
+        <v>629000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1570,8 +1734,12 @@
       <c r="F29">
         <v>75</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29" s="9">
+        <f t="shared" si="1"/>
+        <v>640000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1592,8 +1760,12 @@
       <c r="F30">
         <v>75</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30" s="9">
+        <f t="shared" si="1"/>
+        <v>654000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1614,8 +1786,12 @@
       <c r="F31">
         <v>85</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31" s="9">
+        <f t="shared" si="1"/>
+        <v>665000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1636,8 +1812,12 @@
       <c r="F32">
         <v>85</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32" s="9">
+        <f t="shared" si="1"/>
+        <v>678000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1658,8 +1838,12 @@
       <c r="F33">
         <v>100</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33" s="9">
+        <f t="shared" si="1"/>
+        <v>692000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1680,8 +1864,12 @@
       <c r="F34">
         <v>85</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34" s="9">
+        <f t="shared" si="1"/>
+        <v>706000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1702,8 +1890,12 @@
       <c r="F35">
         <v>100</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G35" s="9">
+        <f t="shared" si="1"/>
+        <v>722000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1724,8 +1916,12 @@
       <c r="F36">
         <v>75</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G36" s="9">
+        <f t="shared" si="1"/>
+        <v>732000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1746,8 +1942,12 @@
       <c r="F37">
         <v>85</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G37" s="9">
+        <f t="shared" si="1"/>
+        <v>741000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1768,8 +1968,12 @@
       <c r="F38">
         <v>75</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G38" s="9">
+        <f t="shared" si="1"/>
+        <v>752000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1790,8 +1994,12 @@
       <c r="F39">
         <v>100</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G39" s="9">
+        <f t="shared" si="1"/>
+        <v>763000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1812,8 +2020,12 @@
       <c r="F40">
         <v>85</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G40" s="9">
+        <f t="shared" si="1"/>
+        <v>777000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1834,8 +2046,12 @@
       <c r="F41">
         <v>85</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G41" s="9">
+        <f t="shared" si="1"/>
+        <v>790000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1856,8 +2072,12 @@
       <c r="F42">
         <v>100</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G42" s="9">
+        <f t="shared" si="1"/>
+        <v>804000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1878,8 +2098,12 @@
       <c r="F43">
         <v>75</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G43" s="9">
+        <f t="shared" si="1"/>
+        <v>817000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1900,8 +2124,12 @@
       <c r="F44">
         <v>75</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G44" s="9">
+        <f t="shared" si="1"/>
+        <v>828000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1922,8 +2150,12 @@
       <c r="F45">
         <v>85</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G45" s="9">
+        <f t="shared" si="1"/>
+        <v>838000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1944,8 +2176,12 @@
       <c r="F46">
         <v>85</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G46" s="9">
+        <f t="shared" si="1"/>
+        <v>852000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1966,8 +2202,12 @@
       <c r="F47">
         <v>100</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G47" s="9">
+        <f t="shared" si="1"/>
+        <v>865000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1988,8 +2228,12 @@
       <c r="F48">
         <v>75</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G48" s="9">
+        <f t="shared" si="1"/>
+        <v>880000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2010,8 +2254,12 @@
       <c r="F49">
         <v>75</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G49" s="9">
+        <f t="shared" si="1"/>
+        <v>892000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2032,8 +2280,12 @@
       <c r="F50">
         <v>85</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G50" s="9">
+        <f t="shared" si="1"/>
+        <v>905000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2054,8 +2306,12 @@
       <c r="F51">
         <v>85</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G51" s="9">
+        <f t="shared" si="1"/>
+        <v>916000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2076,8 +2332,12 @@
       <c r="F52">
         <v>85</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G52" s="9">
+        <f t="shared" si="1"/>
+        <v>929000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2098,8 +2358,12 @@
       <c r="F53">
         <v>75</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G53" s="9">
+        <f t="shared" si="1"/>
+        <v>940000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2120,8 +2384,12 @@
       <c r="F54">
         <v>100</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G54" s="9">
+        <f t="shared" si="1"/>
+        <v>956000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2142,8 +2410,12 @@
       <c r="F55">
         <v>75</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G55" s="9">
+        <f t="shared" si="1"/>
+        <v>969000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2164,8 +2436,12 @@
       <c r="F56">
         <v>75</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G56" s="9">
+        <f t="shared" si="1"/>
+        <v>980000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2186,8 +2462,12 @@
       <c r="F57">
         <v>85</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G57" s="9">
+        <f t="shared" si="1"/>
+        <v>994000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2208,8 +2488,12 @@
       <c r="F58">
         <v>75</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G58" s="9">
+        <f t="shared" si="1"/>
+        <v>1009000</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2230,8 +2514,12 @@
       <c r="F59">
         <v>85</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G59" s="9">
+        <f t="shared" si="1"/>
+        <v>1026000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2252,8 +2540,12 @@
       <c r="F60">
         <v>85</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G60" s="9">
+        <f t="shared" si="1"/>
+        <v>1041000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2273,6 +2565,10 @@
       </c>
       <c r="F61">
         <v>75</v>
+      </c>
+      <c r="G61" s="9">
+        <f t="shared" si="1"/>
+        <v>1049000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>